<commit_message>
UPDATE -- Penambahan Rapel PPH 21 BPJS di penggajian
</commit_message>
<xml_diff>
--- a/public/FORMAT IMPORT DATA PENGGAJIAN.xlsx
+++ b/public/FORMAT IMPORT DATA PENGGAJIAN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itrsup/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/projek/hcm2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FED79D-53E7-7D40-9B77-46C9A08D27BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24015CFA-3C16-564D-8449-90746C841D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="718">
   <si>
     <t>no</t>
   </si>
@@ -2184,6 +2184,9 @@
   </si>
   <si>
     <t>Transportasi</t>
+  </si>
+  <si>
+    <t>Rapel PPH 21 BPJS</t>
   </si>
 </sst>
 </file>
@@ -2904,8 +2907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AQ5" sqref="AQ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2938,7 +2941,8 @@
     <col min="41" max="41" width="15" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="11.6640625" customWidth="1"/>
     <col min="50" max="50" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="14.33203125" customWidth="1"/>
@@ -3079,6 +3083,9 @@
       <c r="AR1" t="s">
         <v>41</v>
       </c>
+      <c r="AT1" s="104" t="s">
+        <v>717</v>
+      </c>
       <c r="AU1" t="s">
         <v>42</v>
       </c>
@@ -3212,7 +3219,9 @@
         <v>0</v>
       </c>
       <c r="AS2" s="55"/>
-      <c r="AT2" s="55"/>
+      <c r="AT2" s="53">
+        <v>100000</v>
+      </c>
       <c r="AU2" s="53">
         <v>255773.32399999999</v>
       </c>
@@ -3346,7 +3355,9 @@
         <v>0</v>
       </c>
       <c r="AS3" s="55"/>
-      <c r="AT3" s="55"/>
+      <c r="AT3" s="53">
+        <v>200000</v>
+      </c>
       <c r="AU3" s="53">
         <v>301653.32400000002</v>
       </c>
@@ -3474,7 +3485,7 @@
         <v>7900</v>
       </c>
       <c r="AS4" s="55"/>
-      <c r="AT4" s="55"/>
+      <c r="AT4" s="53"/>
       <c r="AU4" s="53">
         <v>298160.82400000002</v>
       </c>
@@ -3610,7 +3621,7 @@
         <v>31600</v>
       </c>
       <c r="AS5" s="55"/>
-      <c r="AT5" s="55"/>
+      <c r="AT5" s="53"/>
       <c r="AU5" s="53">
         <v>657347.32400000002</v>
       </c>
@@ -3742,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="AS6" s="55"/>
-      <c r="AT6" s="55"/>
+      <c r="AT6" s="53"/>
       <c r="AU6" s="53">
         <v>299117.32400000002</v>
       </c>
@@ -3870,7 +3881,7 @@
         <v>0</v>
       </c>
       <c r="AS7" s="55"/>
-      <c r="AT7" s="55"/>
+      <c r="AT7" s="53"/>
       <c r="AU7" s="53">
         <v>255927.82399999999</v>
       </c>
@@ -4004,7 +4015,7 @@
         <v>7900</v>
       </c>
       <c r="AS8" s="55"/>
-      <c r="AT8" s="55"/>
+      <c r="AT8" s="53"/>
       <c r="AU8" s="53">
         <v>291603.32400000002</v>
       </c>
@@ -4138,7 +4149,7 @@
         <v>15800</v>
       </c>
       <c r="AS9" s="55"/>
-      <c r="AT9" s="55"/>
+      <c r="AT9" s="53"/>
       <c r="AU9" s="53">
         <v>345203.32400000002</v>
       </c>
@@ -4276,7 +4287,7 @@
         <v>7900</v>
       </c>
       <c r="AS10" s="55"/>
-      <c r="AT10" s="55"/>
+      <c r="AT10" s="53"/>
       <c r="AU10" s="53">
         <v>441685.32400000002</v>
       </c>
@@ -4414,7 +4425,7 @@
         <v>7900</v>
       </c>
       <c r="AS11" s="55"/>
-      <c r="AT11" s="55"/>
+      <c r="AT11" s="53"/>
       <c r="AU11" s="53">
         <v>320600.82400000002</v>
       </c>
@@ -4544,7 +4555,7 @@
         <v>0</v>
       </c>
       <c r="AS12" s="55"/>
-      <c r="AT12" s="55"/>
+      <c r="AT12" s="53"/>
       <c r="AU12" s="53">
         <v>226071.92</v>
       </c>
@@ -4678,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="AS13" s="55"/>
-      <c r="AT13" s="55"/>
+      <c r="AT13" s="53"/>
       <c r="AU13" s="53">
         <v>361703.32400000002</v>
       </c>
@@ -4810,7 +4821,7 @@
         <v>0</v>
       </c>
       <c r="AS14" s="55"/>
-      <c r="AT14" s="55"/>
+      <c r="AT14" s="53"/>
       <c r="AU14" s="53">
         <v>357903.32400000002</v>
       </c>
@@ -4936,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="AS15" s="55"/>
-      <c r="AT15" s="55"/>
+      <c r="AT15" s="53"/>
       <c r="AU15" s="53">
         <v>244501.24299999999</v>
       </c>
@@ -5066,7 +5077,7 @@
         <v>31600</v>
       </c>
       <c r="AS16" s="55"/>
-      <c r="AT16" s="55"/>
+      <c r="AT16" s="53"/>
       <c r="AU16" s="53">
         <v>311953.32400000002</v>
       </c>
@@ -5200,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="AS17" s="55"/>
-      <c r="AT17" s="55"/>
+      <c r="AT17" s="53"/>
       <c r="AU17" s="53">
         <v>255035.82399999999</v>
       </c>
@@ -5330,7 +5341,7 @@
         <v>15800</v>
       </c>
       <c r="AS18" s="55"/>
-      <c r="AT18" s="55"/>
+      <c r="AT18" s="53"/>
       <c r="AU18" s="53">
         <v>269885.82400000002</v>
       </c>
@@ -5462,7 +5473,7 @@
         <v>39500</v>
       </c>
       <c r="AS19" s="55"/>
-      <c r="AT19" s="55"/>
+      <c r="AT19" s="53"/>
       <c r="AU19" s="53">
         <v>285035.82400000002</v>
       </c>
@@ -5592,7 +5603,7 @@
         <v>0</v>
       </c>
       <c r="AS20" s="55"/>
-      <c r="AT20" s="55"/>
+      <c r="AT20" s="53"/>
       <c r="AU20" s="53">
         <v>299609.82400000002</v>
       </c>
@@ -5726,7 +5737,7 @@
         <v>0</v>
       </c>
       <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
+      <c r="AT21" s="53"/>
       <c r="AU21" s="53">
         <v>417435.82400000002</v>
       </c>
@@ -5856,7 +5867,7 @@
         <v>0</v>
       </c>
       <c r="AS22" s="55"/>
-      <c r="AT22" s="55"/>
+      <c r="AT22" s="53"/>
       <c r="AU22" s="53">
         <v>243505.0275</v>
       </c>
@@ -5982,7 +5993,7 @@
         <v>0</v>
       </c>
       <c r="AS23" s="55"/>
-      <c r="AT23" s="55"/>
+      <c r="AT23" s="53"/>
       <c r="AU23" s="53">
         <v>208423.0275</v>
       </c>
@@ -6114,7 +6125,7 @@
         <v>7900</v>
       </c>
       <c r="AS24" s="55"/>
-      <c r="AT24" s="55"/>
+      <c r="AT24" s="53"/>
       <c r="AU24" s="53">
         <v>320642.82400000002</v>
       </c>
@@ -6244,7 +6255,7 @@
         <v>7900</v>
       </c>
       <c r="AS25" s="55"/>
-      <c r="AT25" s="55"/>
+      <c r="AT25" s="53"/>
       <c r="AU25" s="53">
         <v>255810.82399999999</v>
       </c>
@@ -6374,7 +6385,7 @@
         <v>0</v>
       </c>
       <c r="AS26" s="55"/>
-      <c r="AT26" s="55"/>
+      <c r="AT26" s="53"/>
       <c r="AU26" s="53">
         <v>249335.82399999999</v>
       </c>
@@ -6500,7 +6511,7 @@
         <v>0</v>
       </c>
       <c r="AS27" s="55"/>
-      <c r="AT27" s="55"/>
+      <c r="AT27" s="53"/>
       <c r="AU27" s="53">
         <v>234560.82399999999</v>
       </c>
@@ -6628,7 +6639,7 @@
         <v>39500</v>
       </c>
       <c r="AS28" s="55"/>
-      <c r="AT28" s="55"/>
+      <c r="AT28" s="53"/>
       <c r="AU28" s="53">
         <v>282135.82400000002</v>
       </c>
@@ -6760,7 +6771,7 @@
         <v>0</v>
       </c>
       <c r="AS29" s="55"/>
-      <c r="AT29" s="55"/>
+      <c r="AT29" s="53"/>
       <c r="AU29" s="53">
         <v>264060.82400000002</v>
       </c>
@@ -6888,7 +6899,7 @@
         <v>0</v>
       </c>
       <c r="AS30" s="55"/>
-      <c r="AT30" s="55"/>
+      <c r="AT30" s="53"/>
       <c r="AU30" s="53">
         <v>235035.82399999999</v>
       </c>
@@ -7022,7 +7033,7 @@
         <v>7900</v>
       </c>
       <c r="AS31" s="55"/>
-      <c r="AT31" s="55"/>
+      <c r="AT31" s="53"/>
       <c r="AU31" s="53">
         <v>512435.82400000002</v>
       </c>
@@ -7154,7 +7165,7 @@
         <v>7900</v>
       </c>
       <c r="AS32" s="55"/>
-      <c r="AT32" s="55"/>
+      <c r="AT32" s="53"/>
       <c r="AU32" s="53">
         <v>329703.32400000002</v>
       </c>
@@ -7288,7 +7299,7 @@
         <v>126400</v>
       </c>
       <c r="AS33" s="55"/>
-      <c r="AT33" s="55"/>
+      <c r="AT33" s="53"/>
       <c r="AU33" s="53">
         <v>406278.32400000002</v>
       </c>
@@ -7422,7 +7433,7 @@
         <v>39500</v>
       </c>
       <c r="AS34" s="55"/>
-      <c r="AT34" s="55"/>
+      <c r="AT34" s="53"/>
       <c r="AU34" s="53">
         <v>308002.82400000002</v>
       </c>
@@ -7558,7 +7569,7 @@
         <v>0</v>
       </c>
       <c r="AS35" s="55"/>
-      <c r="AT35" s="55"/>
+      <c r="AT35" s="53"/>
       <c r="AU35" s="53">
         <v>356748.32400000002</v>
       </c>
@@ -7684,7 +7695,7 @@
         <v>39500</v>
       </c>
       <c r="AS36" s="55"/>
-      <c r="AT36" s="55"/>
+      <c r="AT36" s="53"/>
       <c r="AU36" s="53">
         <v>265576.104833333</v>
       </c>
@@ -7816,7 +7827,7 @@
         <v>0</v>
       </c>
       <c r="AS37" s="55"/>
-      <c r="AT37" s="55"/>
+      <c r="AT37" s="53"/>
       <c r="AU37" s="53">
         <v>265903.32400000002</v>
       </c>
@@ -7944,7 +7955,7 @@
         <v>0</v>
       </c>
       <c r="AS38" s="55"/>
-      <c r="AT38" s="55"/>
+      <c r="AT38" s="53"/>
       <c r="AU38" s="53">
         <v>272278.32400000002</v>
       </c>
@@ -8078,7 +8089,7 @@
         <v>0</v>
       </c>
       <c r="AS39" s="55"/>
-      <c r="AT39" s="55"/>
+      <c r="AT39" s="53"/>
       <c r="AU39" s="53">
         <v>320500.32400000002</v>
       </c>
@@ -8208,7 +8219,7 @@
         <v>7900</v>
       </c>
       <c r="AS40" s="55"/>
-      <c r="AT40" s="55"/>
+      <c r="AT40" s="53"/>
       <c r="AU40" s="53">
         <v>236753.32399999999</v>
       </c>
@@ -8340,7 +8351,7 @@
         <v>31600</v>
       </c>
       <c r="AS41" s="55"/>
-      <c r="AT41" s="55"/>
+      <c r="AT41" s="53"/>
       <c r="AU41" s="53">
         <v>274235.82400000002</v>
       </c>
@@ -8474,7 +8485,7 @@
         <v>7900</v>
       </c>
       <c r="AS42" s="55"/>
-      <c r="AT42" s="55"/>
+      <c r="AT42" s="53"/>
       <c r="AU42" s="53">
         <v>338278.32400000002</v>
       </c>
@@ -8608,7 +8619,7 @@
         <v>55300</v>
       </c>
       <c r="AS43" s="55"/>
-      <c r="AT43" s="55"/>
+      <c r="AT43" s="53"/>
       <c r="AU43" s="53">
         <v>305953.32400000002</v>
       </c>
@@ -8738,7 +8749,7 @@
         <v>0</v>
       </c>
       <c r="AS44" s="55"/>
-      <c r="AT44" s="55"/>
+      <c r="AT44" s="53"/>
       <c r="AU44" s="53">
         <v>206071.92</v>
       </c>
@@ -8868,7 +8879,7 @@
         <v>126400</v>
       </c>
       <c r="AS45" s="55"/>
-      <c r="AT45" s="55"/>
+      <c r="AT45" s="53"/>
       <c r="AU45" s="53">
         <v>386885.82400000002</v>
       </c>
@@ -9000,7 +9011,7 @@
         <v>31600</v>
       </c>
       <c r="AS46" s="55"/>
-      <c r="AT46" s="55"/>
+      <c r="AT46" s="53"/>
       <c r="AU46" s="53">
         <v>1220461.132</v>
       </c>
@@ -9132,7 +9143,7 @@
         <v>23700</v>
       </c>
       <c r="AS47" s="55"/>
-      <c r="AT47" s="55"/>
+      <c r="AT47" s="53"/>
       <c r="AU47" s="53">
         <v>1631147.132</v>
       </c>
@@ -9260,7 +9271,7 @@
         <v>7900</v>
       </c>
       <c r="AS48" s="55"/>
-      <c r="AT48" s="55"/>
+      <c r="AT48" s="53"/>
       <c r="AU48" s="53">
         <v>831811.13199999998</v>
       </c>
@@ -9390,7 +9401,7 @@
         <v>0</v>
       </c>
       <c r="AS49" s="55"/>
-      <c r="AT49" s="55"/>
+      <c r="AT49" s="53"/>
       <c r="AU49" s="53">
         <v>747411.13199999998</v>
       </c>
@@ -9514,7 +9525,7 @@
         <v>0</v>
       </c>
       <c r="AS50" s="55"/>
-      <c r="AT50" s="55"/>
+      <c r="AT50" s="53"/>
       <c r="AU50" s="53">
         <v>10000</v>
       </c>
@@ -9646,7 +9657,7 @@
         <v>15800</v>
       </c>
       <c r="AS51" s="55"/>
-      <c r="AT51" s="55"/>
+      <c r="AT51" s="53"/>
       <c r="AU51" s="53">
         <v>1248211.132</v>
       </c>
@@ -9782,7 +9793,7 @@
         <v>126400</v>
       </c>
       <c r="AS52" s="55"/>
-      <c r="AT52" s="55"/>
+      <c r="AT52" s="53"/>
       <c r="AU52" s="53">
         <v>1420138.132</v>
       </c>
@@ -9916,7 +9927,7 @@
         <v>0</v>
       </c>
       <c r="AS53" s="55"/>
-      <c r="AT53" s="55"/>
+      <c r="AT53" s="53"/>
       <c r="AU53" s="53">
         <v>1404961.132</v>
       </c>
@@ -10044,7 +10055,7 @@
         <v>15800</v>
       </c>
       <c r="AS54" s="55"/>
-      <c r="AT54" s="55"/>
+      <c r="AT54" s="53"/>
       <c r="AU54" s="53">
         <v>266335.82400000002</v>
       </c>
@@ -10174,7 +10185,7 @@
         <v>7900</v>
       </c>
       <c r="AS55" s="55"/>
-      <c r="AT55" s="55"/>
+      <c r="AT55" s="53"/>
       <c r="AU55" s="53">
         <v>265785.82400000002</v>
       </c>
@@ -10308,7 +10319,7 @@
         <v>126400</v>
       </c>
       <c r="AS56" s="55"/>
-      <c r="AT56" s="55"/>
+      <c r="AT56" s="53"/>
       <c r="AU56" s="53">
         <v>413260.82400000002</v>
       </c>
@@ -10442,7 +10453,7 @@
         <v>7900</v>
       </c>
       <c r="AS57" s="55"/>
-      <c r="AT57" s="55"/>
+      <c r="AT57" s="53"/>
       <c r="AU57" s="53">
         <v>1222836.824</v>
       </c>
@@ -10574,7 +10585,7 @@
         <v>7900</v>
       </c>
       <c r="AS58" s="55"/>
-      <c r="AT58" s="55"/>
+      <c r="AT58" s="53"/>
       <c r="AU58" s="53">
         <v>262935.82400000002</v>
       </c>
@@ -10706,7 +10717,7 @@
         <v>0</v>
       </c>
       <c r="AS59" s="55"/>
-      <c r="AT59" s="55"/>
+      <c r="AT59" s="53"/>
       <c r="AU59" s="53">
         <v>555000</v>
       </c>
@@ -10832,7 +10843,7 @@
         <v>102700</v>
       </c>
       <c r="AS60" s="55"/>
-      <c r="AT60" s="55"/>
+      <c r="AT60" s="53"/>
       <c r="AU60" s="53">
         <v>403485.82400000002</v>
       </c>
@@ -10966,7 +10977,7 @@
         <v>0</v>
       </c>
       <c r="AS61" s="55"/>
-      <c r="AT61" s="55"/>
+      <c r="AT61" s="53"/>
       <c r="AU61" s="53">
         <v>237010.82399999999</v>
       </c>
@@ -11100,7 +11111,7 @@
         <v>15800</v>
       </c>
       <c r="AS62" s="55"/>
-      <c r="AT62" s="55"/>
+      <c r="AT62" s="53"/>
       <c r="AU62" s="53">
         <v>309310.82400000002</v>
       </c>
@@ -11232,7 +11243,7 @@
         <v>0</v>
       </c>
       <c r="AS63" s="55"/>
-      <c r="AT63" s="55"/>
+      <c r="AT63" s="53"/>
       <c r="AU63" s="53">
         <v>237260.82399999999</v>
       </c>
@@ -11358,7 +11369,7 @@
         <v>7900</v>
       </c>
       <c r="AS64" s="55"/>
-      <c r="AT64" s="55"/>
+      <c r="AT64" s="53"/>
       <c r="AU64" s="53">
         <v>314382.82400000002</v>
       </c>
@@ -11490,7 +11501,7 @@
         <v>15800</v>
       </c>
       <c r="AS65" s="55"/>
-      <c r="AT65" s="55"/>
+      <c r="AT65" s="53"/>
       <c r="AU65" s="53">
         <v>323703.32400000002</v>
       </c>
@@ -11616,7 +11627,7 @@
         <v>0</v>
       </c>
       <c r="AS66" s="55"/>
-      <c r="AT66" s="55"/>
+      <c r="AT66" s="53"/>
       <c r="AU66" s="53">
         <v>225535.82399999999</v>
       </c>
@@ -11742,7 +11753,7 @@
         <v>0</v>
       </c>
       <c r="AS67" s="55"/>
-      <c r="AT67" s="55"/>
+      <c r="AT67" s="53"/>
       <c r="AU67" s="53">
         <v>245535.82399999999</v>
       </c>
@@ -11868,7 +11879,7 @@
         <v>0</v>
       </c>
       <c r="AS68" s="55"/>
-      <c r="AT68" s="55"/>
+      <c r="AT68" s="53"/>
       <c r="AU68" s="53">
         <v>245535.82399999999</v>
       </c>
@@ -11994,7 +12005,7 @@
         <v>0</v>
       </c>
       <c r="AS69" s="55"/>
-      <c r="AT69" s="55"/>
+      <c r="AT69" s="53"/>
       <c r="AU69" s="53">
         <v>734111.13199999998</v>
       </c>
@@ -12122,7 +12133,7 @@
         <v>7900</v>
       </c>
       <c r="AS70" s="55"/>
-      <c r="AT70" s="55"/>
+      <c r="AT70" s="53"/>
       <c r="AU70" s="53">
         <v>584203.82400000002</v>
       </c>
@@ -12248,7 +12259,7 @@
         <v>0</v>
       </c>
       <c r="AS71" s="55"/>
-      <c r="AT71" s="55"/>
+      <c r="AT71" s="53"/>
       <c r="AU71" s="53">
         <v>234085.82399999999</v>
       </c>
@@ -12376,7 +12387,7 @@
         <v>126400</v>
       </c>
       <c r="AS72" s="55"/>
-      <c r="AT72" s="55"/>
+      <c r="AT72" s="53"/>
       <c r="AU72" s="53">
         <v>583503.32400000002</v>
       </c>
@@ -12506,7 +12517,7 @@
         <v>0</v>
       </c>
       <c r="AS73" s="55"/>
-      <c r="AT73" s="55"/>
+      <c r="AT73" s="53"/>
       <c r="AU73" s="53">
         <v>1389661.132</v>
       </c>
@@ -12632,7 +12643,7 @@
         <v>0</v>
       </c>
       <c r="AS74" s="55"/>
-      <c r="AT74" s="55"/>
+      <c r="AT74" s="53"/>
       <c r="AU74" s="53">
         <v>293178.32400000002</v>
       </c>
@@ -12760,7 +12771,7 @@
         <v>15800</v>
       </c>
       <c r="AS75" s="55"/>
-      <c r="AT75" s="55"/>
+      <c r="AT75" s="53"/>
       <c r="AU75" s="53">
         <v>325930.32400000002</v>
       </c>
@@ -12886,7 +12897,7 @@
         <v>0</v>
       </c>
       <c r="AS76" s="55"/>
-      <c r="AT76" s="55"/>
+      <c r="AT76" s="53"/>
       <c r="AU76" s="53">
         <v>258835.82399999999</v>
       </c>
@@ -13016,7 +13027,7 @@
         <v>0</v>
       </c>
       <c r="AS77" s="55"/>
-      <c r="AT77" s="55"/>
+      <c r="AT77" s="53"/>
       <c r="AU77" s="53">
         <v>461210.82400000002</v>
       </c>
@@ -13142,7 +13153,7 @@
         <v>0</v>
       </c>
       <c r="AS78" s="55"/>
-      <c r="AT78" s="55"/>
+      <c r="AT78" s="53"/>
       <c r="AU78" s="53">
         <v>225535.82399999999</v>
       </c>
@@ -13266,7 +13277,7 @@
         <v>0</v>
       </c>
       <c r="AS79" s="55"/>
-      <c r="AT79" s="55"/>
+      <c r="AT79" s="53"/>
       <c r="AU79" s="53">
         <v>245535.82399999999</v>
       </c>
@@ -13390,7 +13401,7 @@
         <v>0</v>
       </c>
       <c r="AS80" s="55"/>
-      <c r="AT80" s="55"/>
+      <c r="AT80" s="53"/>
       <c r="AU80" s="53">
         <v>245535.82399999999</v>
       </c>
@@ -13516,7 +13527,7 @@
         <v>23700</v>
       </c>
       <c r="AS81" s="55"/>
-      <c r="AT81" s="55"/>
+      <c r="AT81" s="53"/>
       <c r="AU81" s="53">
         <v>372215.82400000002</v>
       </c>
@@ -13650,7 +13661,7 @@
         <v>126400</v>
       </c>
       <c r="AS82" s="55"/>
-      <c r="AT82" s="55"/>
+      <c r="AT82" s="53"/>
       <c r="AU82" s="53">
         <v>442700.32400000002</v>
       </c>
@@ -13776,7 +13787,7 @@
         <v>63200</v>
       </c>
       <c r="AS83" s="55"/>
-      <c r="AT83" s="55"/>
+      <c r="AT83" s="53"/>
       <c r="AU83" s="53">
         <v>288735.82400000002</v>
       </c>
@@ -13906,7 +13917,7 @@
         <v>126400</v>
       </c>
       <c r="AS84" s="55"/>
-      <c r="AT84" s="55"/>
+      <c r="AT84" s="53"/>
       <c r="AU84" s="53">
         <v>453303.32400000002</v>
       </c>
@@ -14034,7 +14045,7 @@
         <v>0</v>
       </c>
       <c r="AS85" s="55"/>
-      <c r="AT85" s="55"/>
+      <c r="AT85" s="53"/>
       <c r="AU85" s="53">
         <v>226071.92</v>
       </c>
@@ -14162,7 +14173,7 @@
         <v>0</v>
       </c>
       <c r="AS86" s="55"/>
-      <c r="AT86" s="55"/>
+      <c r="AT86" s="53"/>
       <c r="AU86" s="53">
         <v>337903.32400000002</v>
       </c>
@@ -14286,7 +14297,7 @@
         <v>0</v>
       </c>
       <c r="AS87" s="55"/>
-      <c r="AT87" s="55"/>
+      <c r="AT87" s="53"/>
       <c r="AU87" s="53">
         <v>281018.32400000002</v>
       </c>
@@ -14410,7 +14421,7 @@
         <v>7900</v>
       </c>
       <c r="AS88" s="55"/>
-      <c r="AT88" s="55"/>
+      <c r="AT88" s="53"/>
       <c r="AU88" s="53">
         <v>246101.24299999999</v>
       </c>
@@ -14536,7 +14547,7 @@
         <v>31600</v>
       </c>
       <c r="AS89" s="55"/>
-      <c r="AT89" s="55"/>
+      <c r="AT89" s="53"/>
       <c r="AU89" s="53">
         <v>321385.82400000002</v>
       </c>
@@ -14664,7 +14675,7 @@
         <v>0</v>
       </c>
       <c r="AS90" s="55"/>
-      <c r="AT90" s="55"/>
+      <c r="AT90" s="53"/>
       <c r="AU90" s="53">
         <v>290260.82400000002</v>
       </c>
@@ -14790,7 +14801,7 @@
         <v>0</v>
       </c>
       <c r="AS91" s="55"/>
-      <c r="AT91" s="55"/>
+      <c r="AT91" s="53"/>
       <c r="AU91" s="53">
         <v>235510.82399999999</v>
       </c>
@@ -14918,7 +14929,7 @@
         <v>0</v>
       </c>
       <c r="AS92" s="55"/>
-      <c r="AT92" s="55"/>
+      <c r="AT92" s="53"/>
       <c r="AU92" s="53">
         <v>240768.82399999999</v>
       </c>
@@ -15050,7 +15061,7 @@
         <v>63200</v>
       </c>
       <c r="AS93" s="55"/>
-      <c r="AT93" s="55"/>
+      <c r="AT93" s="53"/>
       <c r="AU93" s="53">
         <v>375900.82400000002</v>
       </c>
@@ -15178,7 +15189,7 @@
         <v>39500</v>
       </c>
       <c r="AS94" s="55"/>
-      <c r="AT94" s="55"/>
+      <c r="AT94" s="53"/>
       <c r="AU94" s="53">
         <v>479082.82400000002</v>
       </c>
@@ -15306,7 +15317,7 @@
         <v>0</v>
       </c>
       <c r="AS95" s="55"/>
-      <c r="AT95" s="55"/>
+      <c r="AT95" s="53"/>
       <c r="AU95" s="53">
         <v>244060.82399999999</v>
       </c>
@@ -15434,7 +15445,7 @@
         <v>0</v>
       </c>
       <c r="AS96" s="55"/>
-      <c r="AT96" s="55"/>
+      <c r="AT96" s="53"/>
       <c r="AU96" s="53">
         <v>267164.32400000002</v>
       </c>
@@ -15562,7 +15573,7 @@
         <v>31600</v>
       </c>
       <c r="AS97" s="55"/>
-      <c r="AT97" s="55"/>
+      <c r="AT97" s="53"/>
       <c r="AU97" s="53">
         <v>284260.82400000002</v>
       </c>
@@ -15688,7 +15699,7 @@
         <v>0</v>
       </c>
       <c r="AS98" s="55"/>
-      <c r="AT98" s="55"/>
+      <c r="AT98" s="53"/>
       <c r="AU98" s="53">
         <v>223018.32399999999</v>
       </c>
@@ -15812,7 +15823,7 @@
         <v>0</v>
       </c>
       <c r="AS99" s="55"/>
-      <c r="AT99" s="55"/>
+      <c r="AT99" s="53"/>
       <c r="AU99" s="53">
         <v>250785.82399999999</v>
       </c>
@@ -15938,7 +15949,7 @@
         <v>39500</v>
       </c>
       <c r="AS100" s="55"/>
-      <c r="AT100" s="55"/>
+      <c r="AT100" s="53"/>
       <c r="AU100" s="53">
         <v>521610.82400000002</v>
       </c>
@@ -16066,7 +16077,7 @@
         <v>0</v>
       </c>
       <c r="AS101" s="55"/>
-      <c r="AT101" s="55"/>
+      <c r="AT101" s="53"/>
       <c r="AU101" s="53">
         <v>238835.82399999999</v>
       </c>
@@ -16194,7 +16205,7 @@
         <v>0</v>
       </c>
       <c r="AS102" s="55"/>
-      <c r="AT102" s="55"/>
+      <c r="AT102" s="53"/>
       <c r="AU102" s="53">
         <v>300285.82400000002</v>
       </c>
@@ -16322,7 +16333,7 @@
         <v>15800</v>
       </c>
       <c r="AS103" s="55"/>
-      <c r="AT103" s="55"/>
+      <c r="AT103" s="53"/>
       <c r="AU103" s="53">
         <v>496737.82400000002</v>
       </c>
@@ -16452,7 +16463,7 @@
         <v>0</v>
       </c>
       <c r="AS104" s="55"/>
-      <c r="AT104" s="55"/>
+      <c r="AT104" s="53"/>
       <c r="AU104" s="53">
         <v>300710.82400000002</v>
       </c>
@@ -16580,7 +16591,7 @@
         <v>126400</v>
       </c>
       <c r="AS105" s="55"/>
-      <c r="AT105" s="55"/>
+      <c r="AT105" s="53"/>
       <c r="AU105" s="53">
         <v>395923.32400000002</v>
       </c>
@@ -16706,7 +16717,7 @@
         <v>102700</v>
       </c>
       <c r="AS106" s="55"/>
-      <c r="AT106" s="55"/>
+      <c r="AT106" s="53"/>
       <c r="AU106" s="53">
         <v>372223.32400000002</v>
       </c>
@@ -16834,7 +16845,7 @@
         <v>0</v>
       </c>
       <c r="AS107" s="55"/>
-      <c r="AT107" s="55"/>
+      <c r="AT107" s="53"/>
       <c r="AU107" s="53">
         <v>1087361.132</v>
       </c>
@@ -16962,7 +16973,7 @@
         <v>0</v>
       </c>
       <c r="AS108" s="55"/>
-      <c r="AT108" s="55"/>
+      <c r="AT108" s="53"/>
       <c r="AU108" s="53">
         <v>480685.82400000002</v>
       </c>
@@ -17090,7 +17101,7 @@
         <v>47400</v>
       </c>
       <c r="AS109" s="55"/>
-      <c r="AT109" s="55"/>
+      <c r="AT109" s="53"/>
       <c r="AU109" s="53">
         <v>307103.32400000002</v>
       </c>
@@ -17218,7 +17229,7 @@
         <v>0</v>
       </c>
       <c r="AS110" s="55"/>
-      <c r="AT110" s="55"/>
+      <c r="AT110" s="53"/>
       <c r="AU110" s="53">
         <v>241685.82399999999</v>
       </c>
@@ -17344,7 +17355,7 @@
         <v>23700</v>
       </c>
       <c r="AS111" s="55"/>
-      <c r="AT111" s="55"/>
+      <c r="AT111" s="53"/>
       <c r="AU111" s="53">
         <v>267760.82400000002</v>
       </c>
@@ -17476,7 +17487,7 @@
         <v>94800</v>
       </c>
       <c r="AS112" s="55"/>
-      <c r="AT112" s="55"/>
+      <c r="AT112" s="53"/>
       <c r="AU112" s="53">
         <v>363953.32400000002</v>
       </c>
@@ -17602,7 +17613,7 @@
         <v>0</v>
       </c>
       <c r="AS113" s="55"/>
-      <c r="AT113" s="55"/>
+      <c r="AT113" s="53"/>
       <c r="AU113" s="53">
         <v>536674.13199999998</v>
       </c>
@@ -17728,7 +17739,7 @@
         <v>7900</v>
       </c>
       <c r="AS114" s="55"/>
-      <c r="AT114" s="55"/>
+      <c r="AT114" s="53"/>
       <c r="AU114" s="53">
         <v>303590.82400000002</v>
       </c>
@@ -17858,7 +17869,7 @@
         <v>126400</v>
       </c>
       <c r="AS115" s="55"/>
-      <c r="AT115" s="55"/>
+      <c r="AT115" s="53"/>
       <c r="AU115" s="53">
         <v>427611.82400000002</v>
       </c>
@@ -17986,7 +17997,7 @@
         <v>23700</v>
       </c>
       <c r="AS116" s="55"/>
-      <c r="AT116" s="55"/>
+      <c r="AT116" s="53"/>
       <c r="AU116" s="53">
         <v>414251.32400000002</v>
       </c>
@@ -18112,7 +18123,7 @@
         <v>0</v>
       </c>
       <c r="AS117" s="55"/>
-      <c r="AT117" s="55"/>
+      <c r="AT117" s="53"/>
       <c r="AU117" s="53">
         <v>253943.32399999999</v>
       </c>
@@ -18236,7 +18247,7 @@
         <v>0</v>
       </c>
       <c r="AS118" s="55"/>
-      <c r="AT118" s="55"/>
+      <c r="AT118" s="53"/>
       <c r="AU118" s="53">
         <v>288264.32400000002</v>
       </c>
@@ -18360,7 +18371,7 @@
         <v>0</v>
       </c>
       <c r="AS119" s="55"/>
-      <c r="AT119" s="55"/>
+      <c r="AT119" s="53"/>
       <c r="AU119" s="53">
         <v>234418.32399999999</v>
       </c>
@@ -18486,7 +18497,7 @@
         <v>0</v>
       </c>
       <c r="AS120" s="55"/>
-      <c r="AT120" s="55"/>
+      <c r="AT120" s="53"/>
       <c r="AU120" s="53">
         <v>259643.32399999999</v>
       </c>
@@ -18610,7 +18621,7 @@
         <v>0</v>
       </c>
       <c r="AS121" s="55"/>
-      <c r="AT121" s="55"/>
+      <c r="AT121" s="53"/>
       <c r="AU121" s="53">
         <v>223018.32399999999</v>
       </c>
@@ -18734,7 +18745,7 @@
         <v>0</v>
       </c>
       <c r="AS122" s="55"/>
-      <c r="AT122" s="55"/>
+      <c r="AT122" s="53"/>
       <c r="AU122" s="53">
         <v>300844.32400000002</v>
       </c>
@@ -18858,7 +18869,7 @@
         <v>0</v>
       </c>
       <c r="AS123" s="55"/>
-      <c r="AT123" s="55"/>
+      <c r="AT123" s="53"/>
       <c r="AU123" s="53">
         <v>242065.32399999999</v>
       </c>
@@ -18982,7 +18993,7 @@
         <v>0</v>
       </c>
       <c r="AS124" s="55"/>
-      <c r="AT124" s="55"/>
+      <c r="AT124" s="53"/>
       <c r="AU124" s="53">
         <v>241068.32399999999</v>
       </c>
@@ -19108,7 +19119,7 @@
         <v>0</v>
       </c>
       <c r="AS125" s="55"/>
-      <c r="AT125" s="55"/>
+      <c r="AT125" s="53"/>
       <c r="AU125" s="53">
         <v>226071.92</v>
       </c>
@@ -19228,7 +19239,7 @@
         <v>0</v>
       </c>
       <c r="AS126" s="55"/>
-      <c r="AT126" s="55"/>
+      <c r="AT126" s="53"/>
       <c r="AU126" s="53">
         <v>233943.32399999999</v>
       </c>
@@ -19352,7 +19363,7 @@
         <v>0</v>
       </c>
       <c r="AS127" s="55"/>
-      <c r="AT127" s="55"/>
+      <c r="AT127" s="53"/>
       <c r="AU127" s="53">
         <v>256318.32399999999</v>
       </c>
@@ -19476,7 +19487,7 @@
         <v>0</v>
       </c>
       <c r="AS128" s="55"/>
-      <c r="AT128" s="55"/>
+      <c r="AT128" s="53"/>
       <c r="AU128" s="53">
         <v>236318.32399999999</v>
       </c>
@@ -19602,7 +19613,7 @@
         <v>0</v>
       </c>
       <c r="AS129" s="55"/>
-      <c r="AT129" s="55"/>
+      <c r="AT129" s="53"/>
       <c r="AU129" s="53">
         <v>271043.32400000002</v>
       </c>
@@ -19728,7 +19739,7 @@
         <v>0</v>
       </c>
       <c r="AS130" s="55"/>
-      <c r="AT130" s="55"/>
+      <c r="AT130" s="53"/>
       <c r="AU130" s="53">
         <v>316293.32400000002</v>
       </c>
@@ -19852,7 +19863,7 @@
         <v>0</v>
       </c>
       <c r="AS131" s="55"/>
-      <c r="AT131" s="55"/>
+      <c r="AT131" s="53"/>
       <c r="AU131" s="53">
         <v>244393.32399999999</v>
       </c>
@@ -19980,7 +19991,7 @@
         <v>7900</v>
       </c>
       <c r="AS132" s="55"/>
-      <c r="AT132" s="55"/>
+      <c r="AT132" s="53"/>
       <c r="AU132" s="53">
         <v>932591.32400000002</v>
       </c>
@@ -20104,7 +20115,7 @@
         <v>31600</v>
       </c>
       <c r="AS133" s="55"/>
-      <c r="AT133" s="55"/>
+      <c r="AT133" s="53"/>
       <c r="AU133" s="53">
         <v>265543.32400000002</v>
       </c>
@@ -20230,7 +20241,7 @@
         <v>0</v>
       </c>
       <c r="AS134" s="55"/>
-      <c r="AT134" s="55"/>
+      <c r="AT134" s="53"/>
       <c r="AU134" s="53">
         <v>234893.32399999999</v>
       </c>
@@ -20356,7 +20367,7 @@
         <v>23700</v>
       </c>
       <c r="AS135" s="55"/>
-      <c r="AT135" s="55"/>
+      <c r="AT135" s="53"/>
       <c r="AU135" s="53">
         <v>285718.32400000002</v>
       </c>
@@ -20484,7 +20495,7 @@
         <v>0</v>
       </c>
       <c r="AS136" s="55"/>
-      <c r="AT136" s="55"/>
+      <c r="AT136" s="53"/>
       <c r="AU136" s="53">
         <v>482268.32400000002</v>
       </c>
@@ -20608,7 +20619,7 @@
         <v>0</v>
       </c>
       <c r="AS137" s="55"/>
-      <c r="AT137" s="55"/>
+      <c r="AT137" s="53"/>
       <c r="AU137" s="53">
         <v>239643.32399999999</v>
       </c>
@@ -20732,7 +20743,7 @@
         <v>0</v>
       </c>
       <c r="AS138" s="55"/>
-      <c r="AT138" s="55"/>
+      <c r="AT138" s="53"/>
       <c r="AU138" s="53">
         <v>232518.32399999999</v>
       </c>
@@ -20856,7 +20867,7 @@
         <v>23700</v>
       </c>
       <c r="AS139" s="55"/>
-      <c r="AT139" s="55"/>
+      <c r="AT139" s="53"/>
       <c r="AU139" s="53">
         <v>306143.32400000002</v>
       </c>
@@ -20984,7 +20995,7 @@
         <v>7900</v>
       </c>
       <c r="AS140" s="55"/>
-      <c r="AT140" s="55"/>
+      <c r="AT140" s="53"/>
       <c r="AU140" s="53">
         <v>355818.32400000002</v>
       </c>
@@ -21112,7 +21123,7 @@
         <v>0</v>
       </c>
       <c r="AS141" s="55"/>
-      <c r="AT141" s="55"/>
+      <c r="AT141" s="53"/>
       <c r="AU141" s="53">
         <v>271018.32400000002</v>
       </c>
@@ -21234,7 +21245,7 @@
         <v>7900</v>
       </c>
       <c r="AS142" s="55"/>
-      <c r="AT142" s="55"/>
+      <c r="AT142" s="53"/>
       <c r="AU142" s="53">
         <v>213971.92</v>
       </c>
@@ -21358,7 +21369,7 @@
         <v>0</v>
       </c>
       <c r="AS143" s="55"/>
-      <c r="AT143" s="55"/>
+      <c r="AT143" s="53"/>
       <c r="AU143" s="53">
         <v>250143.32399999999</v>
       </c>
@@ -21484,7 +21495,7 @@
         <v>0</v>
       </c>
       <c r="AS144" s="55"/>
-      <c r="AT144" s="55"/>
+      <c r="AT144" s="53"/>
       <c r="AU144" s="53">
         <v>270093.32400000002</v>
       </c>
@@ -21610,7 +21621,7 @@
         <v>0</v>
       </c>
       <c r="AS145" s="55"/>
-      <c r="AT145" s="55"/>
+      <c r="AT145" s="53"/>
       <c r="AU145" s="53">
         <v>312022.32400000002</v>
       </c>
@@ -21736,7 +21747,7 @@
         <v>0</v>
       </c>
       <c r="AS146" s="55"/>
-      <c r="AT146" s="55"/>
+      <c r="AT146" s="53"/>
       <c r="AU146" s="53">
         <v>256071.92</v>
       </c>
@@ -21862,7 +21873,7 @@
         <v>0</v>
       </c>
       <c r="AS147" s="55"/>
-      <c r="AT147" s="55"/>
+      <c r="AT147" s="53"/>
       <c r="AU147" s="53">
         <v>271118.32400000002</v>
       </c>
@@ -21988,7 +21999,7 @@
         <v>0</v>
       </c>
       <c r="AS148" s="55"/>
-      <c r="AT148" s="55"/>
+      <c r="AT148" s="53"/>
       <c r="AU148" s="53">
         <v>259168.32399999999</v>
       </c>
@@ -22114,7 +22125,7 @@
         <v>0</v>
       </c>
       <c r="AS149" s="55"/>
-      <c r="AT149" s="55"/>
+      <c r="AT149" s="53"/>
       <c r="AU149" s="53">
         <v>247768.32399999999</v>
       </c>
@@ -22238,7 +22249,7 @@
         <v>0</v>
       </c>
       <c r="AS150" s="55"/>
-      <c r="AT150" s="55"/>
+      <c r="AT150" s="53"/>
       <c r="AU150" s="53">
         <v>496085.631692308</v>
       </c>
@@ -22362,7 +22373,7 @@
         <v>7900</v>
       </c>
       <c r="AS151" s="55"/>
-      <c r="AT151" s="55"/>
+      <c r="AT151" s="53"/>
       <c r="AU151" s="53">
         <v>288796.32400000002</v>
       </c>
@@ -22484,7 +22495,7 @@
         <v>39500</v>
       </c>
       <c r="AS152" s="55"/>
-      <c r="AT152" s="55"/>
+      <c r="AT152" s="53"/>
       <c r="AU152" s="53">
         <v>324268.32400000002</v>
       </c>
@@ -22612,7 +22623,7 @@
         <v>47400</v>
       </c>
       <c r="AS153" s="55"/>
-      <c r="AT153" s="55"/>
+      <c r="AT153" s="53"/>
       <c r="AU153" s="53">
         <v>290418.32400000002</v>
       </c>
@@ -22736,7 +22747,7 @@
         <v>0</v>
       </c>
       <c r="AS154" s="55"/>
-      <c r="AT154" s="55"/>
+      <c r="AT154" s="53"/>
       <c r="AU154" s="53">
         <v>296768.32400000002</v>
       </c>
@@ -22860,7 +22871,7 @@
         <v>0</v>
       </c>
       <c r="AS155" s="55"/>
-      <c r="AT155" s="55"/>
+      <c r="AT155" s="53"/>
       <c r="AU155" s="53">
         <v>257268.32399999999</v>
       </c>
@@ -22984,7 +22995,7 @@
         <v>0</v>
       </c>
       <c r="AS156" s="55"/>
-      <c r="AT156" s="55"/>
+      <c r="AT156" s="53"/>
       <c r="AU156" s="53">
         <v>453768.32400000002</v>
       </c>
@@ -23108,7 +23119,7 @@
         <v>0</v>
       </c>
       <c r="AS157" s="82"/>
-      <c r="AT157" s="82"/>
+      <c r="AT157" s="53"/>
       <c r="AU157" s="85">
         <v>246948.72899999999</v>
       </c>
@@ -23234,7 +23245,7 @@
         <v>0</v>
       </c>
       <c r="AS158" s="55"/>
-      <c r="AT158" s="55"/>
+      <c r="AT158" s="53"/>
       <c r="AU158" s="53">
         <v>256071.92</v>
       </c>
@@ -23356,7 +23367,7 @@
         <v>7900</v>
       </c>
       <c r="AS159" s="55"/>
-      <c r="AT159" s="55"/>
+      <c r="AT159" s="53"/>
       <c r="AU159" s="53">
         <v>213971.92</v>
       </c>
@@ -23468,7 +23479,7 @@
         <v>47400</v>
       </c>
       <c r="AS160" s="55"/>
-      <c r="AT160" s="55"/>
+      <c r="AT160" s="53"/>
       <c r="AU160" s="53">
         <v>241901.24299999999</v>
       </c>
@@ -23598,7 +23609,7 @@
         <v>0</v>
       </c>
       <c r="AS161" s="55"/>
-      <c r="AT161" s="55"/>
+      <c r="AT161" s="53"/>
       <c r="AU161" s="53">
         <v>254712.03649999999</v>
       </c>
@@ -23724,7 +23735,7 @@
         <v>0</v>
       </c>
       <c r="AS162" s="55"/>
-      <c r="AT162" s="55"/>
+      <c r="AT162" s="53"/>
       <c r="AU162" s="53">
         <v>226071.92</v>
       </c>
@@ -23850,7 +23861,7 @@
         <v>0</v>
       </c>
       <c r="AS163" s="55"/>
-      <c r="AT163" s="55"/>
+      <c r="AT163" s="53"/>
       <c r="AU163" s="53">
         <v>207692.68650000001</v>
       </c>
@@ -23972,7 +23983,7 @@
         <v>0</v>
       </c>
       <c r="AS164" s="55"/>
-      <c r="AT164" s="55"/>
+      <c r="AT164" s="53"/>
       <c r="AU164" s="53">
         <v>206071.92</v>
       </c>
@@ -24096,7 +24107,7 @@
         <v>0</v>
       </c>
       <c r="AS165" s="55"/>
-      <c r="AT165" s="55"/>
+      <c r="AT165" s="53"/>
       <c r="AU165" s="53">
         <v>234989.03649999999</v>
       </c>
@@ -24224,7 +24235,7 @@
         <v>0</v>
       </c>
       <c r="AS166" s="55"/>
-      <c r="AT166" s="55"/>
+      <c r="AT166" s="53"/>
       <c r="AU166" s="53">
         <v>262673.72899999999</v>
       </c>
@@ -24348,7 +24359,7 @@
         <v>7900</v>
       </c>
       <c r="AS167" s="55"/>
-      <c r="AT167" s="55"/>
+      <c r="AT167" s="53"/>
       <c r="AU167" s="53">
         <v>244567.68650000001</v>
       </c>
@@ -24480,7 +24491,7 @@
         <v>0</v>
       </c>
       <c r="AS168" s="55"/>
-      <c r="AT168" s="55"/>
+      <c r="AT168" s="53"/>
       <c r="AU168" s="53">
         <v>374842.68650000001</v>
       </c>
@@ -24606,7 +24617,7 @@
         <v>0</v>
       </c>
       <c r="AS169" s="55"/>
-      <c r="AT169" s="55"/>
+      <c r="AT169" s="53"/>
       <c r="AU169" s="53">
         <v>230017.68650000001</v>
       </c>
@@ -24738,7 +24749,7 @@
         <v>0</v>
       </c>
       <c r="AS170" s="55"/>
-      <c r="AT170" s="55"/>
+      <c r="AT170" s="53"/>
       <c r="AU170" s="53">
         <v>1829351.132</v>
       </c>
@@ -24862,7 +24873,7 @@
         <v>0</v>
       </c>
       <c r="AS171" s="55"/>
-      <c r="AT171" s="55"/>
+      <c r="AT171" s="53"/>
       <c r="AU171" s="53">
         <v>226071.92</v>
       </c>
@@ -24972,7 +24983,7 @@
         <v>0</v>
       </c>
       <c r="AS172" s="55"/>
-      <c r="AT172" s="55"/>
+      <c r="AT172" s="53"/>
       <c r="AU172" s="53">
         <v>724381.13199999998</v>
       </c>
@@ -25094,7 +25105,7 @@
         <v>39500</v>
       </c>
       <c r="AS173" s="55"/>
-      <c r="AT173" s="55"/>
+      <c r="AT173" s="53"/>
       <c r="AU173" s="53">
         <v>264039.03649999999</v>
       </c>
@@ -25222,7 +25233,7 @@
         <v>15800</v>
       </c>
       <c r="AS174" s="55"/>
-      <c r="AT174" s="55"/>
+      <c r="AT174" s="53"/>
       <c r="AU174" s="53">
         <v>236539.03649999999</v>
       </c>
@@ -25350,7 +25361,7 @@
         <v>0</v>
       </c>
       <c r="AS175" s="55"/>
-      <c r="AT175" s="55"/>
+      <c r="AT175" s="53"/>
       <c r="AU175" s="53">
         <v>275742.68650000001</v>
       </c>
@@ -25478,7 +25489,7 @@
         <v>0</v>
       </c>
       <c r="AS176" s="55"/>
-      <c r="AT176" s="55"/>
+      <c r="AT176" s="53"/>
       <c r="AU176" s="53">
         <v>246914.03649999999</v>
       </c>
@@ -25604,7 +25615,7 @@
         <v>0</v>
       </c>
       <c r="AS177" s="55"/>
-      <c r="AT177" s="55"/>
+      <c r="AT177" s="53"/>
       <c r="AU177" s="53">
         <v>225489.03649999999</v>
       </c>
@@ -25732,7 +25743,7 @@
         <v>0</v>
       </c>
       <c r="AS178" s="55"/>
-      <c r="AT178" s="55"/>
+      <c r="AT178" s="53"/>
       <c r="AU178" s="53">
         <v>238617.68650000001</v>
       </c>
@@ -25860,7 +25871,7 @@
         <v>0</v>
       </c>
       <c r="AS179" s="55"/>
-      <c r="AT179" s="55"/>
+      <c r="AT179" s="53"/>
       <c r="AU179" s="53">
         <v>239092.68650000001</v>
       </c>
@@ -25984,7 +25995,7 @@
         <v>0</v>
       </c>
       <c r="AS180" s="55"/>
-      <c r="AT180" s="55"/>
+      <c r="AT180" s="53"/>
       <c r="AU180" s="53">
         <v>233089.03649999999</v>
       </c>
@@ -26096,7 +26107,7 @@
         <v>110600</v>
       </c>
       <c r="AS181" s="55"/>
-      <c r="AT181" s="55"/>
+      <c r="AT181" s="53"/>
       <c r="AU181" s="53">
         <v>321839.03649999999</v>
       </c>
@@ -26208,7 +26219,7 @@
         <v>0</v>
       </c>
       <c r="AS182" s="55"/>
-      <c r="AT182" s="55"/>
+      <c r="AT182" s="53"/>
       <c r="AU182" s="53">
         <v>253564.03649999999</v>
       </c>
@@ -26322,7 +26333,7 @@
         <v>15800</v>
       </c>
       <c r="AS183" s="55"/>
-      <c r="AT183" s="55"/>
+      <c r="AT183" s="53"/>
       <c r="AU183" s="53">
         <v>281789.03649999999</v>
       </c>
@@ -26436,7 +26447,7 @@
         <v>7900</v>
       </c>
       <c r="AS184" s="55"/>
-      <c r="AT184" s="55"/>
+      <c r="AT184" s="53"/>
       <c r="AU184" s="53">
         <v>314708.03649999999</v>
       </c>
@@ -26550,7 +26561,7 @@
         <v>0</v>
       </c>
       <c r="AS185" s="55"/>
-      <c r="AT185" s="55"/>
+      <c r="AT185" s="53"/>
       <c r="AU185" s="53">
         <v>223114.03649999999</v>
       </c>
@@ -26662,7 +26673,7 @@
         <v>0</v>
       </c>
       <c r="AS186" s="55"/>
-      <c r="AT186" s="55"/>
+      <c r="AT186" s="53"/>
       <c r="AU186" s="53">
         <v>243589.03649999999</v>
       </c>
@@ -26776,7 +26787,7 @@
         <v>0</v>
       </c>
       <c r="AS187" s="55"/>
-      <c r="AT187" s="55"/>
+      <c r="AT187" s="53"/>
       <c r="AU187" s="53">
         <v>253089.03649999999</v>
       </c>
@@ -26890,7 +26901,7 @@
         <v>0</v>
       </c>
       <c r="AS188" s="55"/>
-      <c r="AT188" s="55"/>
+      <c r="AT188" s="53"/>
       <c r="AU188" s="53">
         <v>270187.03649999999</v>
       </c>
@@ -27002,7 +27013,7 @@
         <v>0</v>
       </c>
       <c r="AS189" s="55"/>
-      <c r="AT189" s="55"/>
+      <c r="AT189" s="53"/>
       <c r="AU189" s="53">
         <v>217513.68650000001</v>
       </c>
@@ -27110,7 +27121,7 @@
         <v>7900</v>
       </c>
       <c r="AS190" s="55"/>
-      <c r="AT190" s="55"/>
+      <c r="AT190" s="53"/>
       <c r="AU190" s="53">
         <v>227942.68650000001</v>
       </c>
@@ -27224,7 +27235,7 @@
         <v>0</v>
       </c>
       <c r="AS191" s="55"/>
-      <c r="AT191" s="55"/>
+      <c r="AT191" s="53"/>
       <c r="AU191" s="53">
         <v>209117.68650000001</v>
       </c>
@@ -27334,7 +27345,7 @@
         <v>7900</v>
       </c>
       <c r="AS192" s="55"/>
-      <c r="AT192" s="55"/>
+      <c r="AT192" s="53"/>
       <c r="AU192" s="53">
         <v>229842.68650000001</v>
       </c>
@@ -27446,7 +27457,7 @@
         <v>0</v>
       </c>
       <c r="AS193" s="55"/>
-      <c r="AT193" s="55"/>
+      <c r="AT193" s="53"/>
       <c r="AU193" s="53">
         <v>211239.03649999999</v>
       </c>
@@ -27554,7 +27565,7 @@
         <v>0</v>
       </c>
       <c r="AS194" s="55"/>
-      <c r="AT194" s="55"/>
+      <c r="AT194" s="53"/>
       <c r="AU194" s="53">
         <v>226439.03649999999</v>
       </c>
@@ -27668,7 +27679,7 @@
         <v>0</v>
       </c>
       <c r="AS195" s="55"/>
-      <c r="AT195" s="55"/>
+      <c r="AT195" s="53"/>
       <c r="AU195" s="53">
         <v>231239.03649999999</v>
       </c>
@@ -27776,7 +27787,7 @@
         <v>0</v>
       </c>
       <c r="AS196" s="55"/>
-      <c r="AT196" s="55"/>
+      <c r="AT196" s="53"/>
       <c r="AU196" s="53">
         <v>224539.03649999999</v>
       </c>
@@ -27888,7 +27899,7 @@
         <v>0</v>
       </c>
       <c r="AS197" s="55"/>
-      <c r="AT197" s="55"/>
+      <c r="AT197" s="53"/>
       <c r="AU197" s="53">
         <v>221214.03649999999</v>
       </c>
@@ -28000,7 +28011,7 @@
         <v>7900</v>
       </c>
       <c r="AS198" s="55"/>
-      <c r="AT198" s="55"/>
+      <c r="AT198" s="53"/>
       <c r="AU198" s="53">
         <v>241717.68650000001</v>
       </c>
@@ -28116,7 +28127,7 @@
         <v>0</v>
       </c>
       <c r="AS199" s="55"/>
-      <c r="AT199" s="55"/>
+      <c r="AT199" s="53"/>
       <c r="AU199" s="53">
         <v>241214.03649999999</v>
       </c>
@@ -28230,7 +28241,7 @@
         <v>0</v>
       </c>
       <c r="AS200" s="55"/>
-      <c r="AT200" s="55"/>
+      <c r="AT200" s="53"/>
       <c r="AU200" s="53">
         <v>243628.03400000001</v>
       </c>
@@ -28342,7 +28353,7 @@
         <v>0</v>
       </c>
       <c r="AS201" s="55"/>
-      <c r="AT201" s="55"/>
+      <c r="AT201" s="53"/>
       <c r="AU201" s="53">
         <v>229289.03649999999</v>
       </c>
@@ -28456,7 +28467,7 @@
         <v>0</v>
       </c>
       <c r="AS202" s="56"/>
-      <c r="AT202" s="56"/>
+      <c r="AT202" s="53"/>
       <c r="AU202" s="56">
         <v>263306.95150000002</v>
       </c>
@@ -28570,7 +28581,7 @@
         <v>7900</v>
       </c>
       <c r="AS203" s="55"/>
-      <c r="AT203" s="55"/>
+      <c r="AT203" s="53"/>
       <c r="AU203" s="53">
         <v>668497.68649999995</v>
       </c>
@@ -28682,7 +28693,7 @@
         <v>31600</v>
       </c>
       <c r="AS204" s="55"/>
-      <c r="AT204" s="55"/>
+      <c r="AT204" s="53"/>
       <c r="AU204" s="53">
         <v>254714.03649999999</v>
       </c>
@@ -28798,7 +28809,7 @@
         <v>0</v>
       </c>
       <c r="AS205" s="55"/>
-      <c r="AT205" s="55"/>
+      <c r="AT205" s="53"/>
       <c r="AU205" s="53">
         <v>259517.68650000001</v>
       </c>
@@ -28910,7 +28921,7 @@
         <v>0</v>
       </c>
       <c r="AS206" s="55"/>
-      <c r="AT206" s="55"/>
+      <c r="AT206" s="53"/>
       <c r="AU206" s="53">
         <v>503661.13199999998</v>
       </c>
@@ -29020,7 +29031,7 @@
         <v>7900</v>
       </c>
       <c r="AS207" s="55"/>
-      <c r="AT207" s="55"/>
+      <c r="AT207" s="53"/>
       <c r="AU207" s="53">
         <v>217492.68650000001</v>
       </c>
@@ -29134,7 +29145,7 @@
         <v>0</v>
       </c>
       <c r="AS208" s="55"/>
-      <c r="AT208" s="55"/>
+      <c r="AT208" s="53"/>
       <c r="AU208" s="53">
         <v>256889.03649999999</v>
       </c>
@@ -29246,7 +29257,7 @@
         <v>0</v>
       </c>
       <c r="AS209" s="55"/>
-      <c r="AT209" s="55"/>
+      <c r="AT209" s="53"/>
       <c r="AU209" s="53">
         <v>225964.03649999999</v>
       </c>
@@ -29358,7 +29369,7 @@
         <v>0</v>
       </c>
       <c r="AS210" s="55"/>
-      <c r="AT210" s="55"/>
+      <c r="AT210" s="53"/>
       <c r="AU210" s="53">
         <v>510661.13199999998</v>
       </c>
@@ -29468,7 +29479,7 @@
         <v>0</v>
       </c>
       <c r="AS211" s="55"/>
-      <c r="AT211" s="55"/>
+      <c r="AT211" s="53"/>
       <c r="AU211" s="53">
         <v>471661.13199999998</v>
       </c>
@@ -29576,7 +29587,7 @@
         <v>0</v>
       </c>
       <c r="AS212" s="55"/>
-      <c r="AT212" s="55"/>
+      <c r="AT212" s="53"/>
       <c r="AU212" s="53">
         <v>206071.92</v>
       </c>
@@ -29684,7 +29695,7 @@
         <v>0</v>
       </c>
       <c r="AS213" s="55"/>
-      <c r="AT213" s="55"/>
+      <c r="AT213" s="53"/>
       <c r="AU213" s="53">
         <v>217192.68650000001</v>
       </c>
@@ -29794,7 +29805,7 @@
         <v>0</v>
       </c>
       <c r="AS214" s="55"/>
-      <c r="AT214" s="55"/>
+      <c r="AT214" s="53"/>
       <c r="AU214" s="53">
         <v>469768.32400000002</v>
       </c>
@@ -29904,7 +29915,7 @@
         <v>0</v>
       </c>
       <c r="AS215" s="55"/>
-      <c r="AT215" s="55"/>
+      <c r="AT215" s="53"/>
       <c r="AU215" s="53">
         <v>256268.32399999999</v>
       </c>
@@ -30014,7 +30025,7 @@
         <v>0</v>
       </c>
       <c r="AS216" s="55"/>
-      <c r="AT216" s="55"/>
+      <c r="AT216" s="53"/>
       <c r="AU216" s="53">
         <v>504706.58654545498</v>
       </c>
@@ -30128,7 +30139,7 @@
         <v>0</v>
       </c>
       <c r="AS217" s="55"/>
-      <c r="AT217" s="55"/>
+      <c r="AT217" s="53"/>
       <c r="AU217" s="53">
         <v>249289.03649999999</v>
       </c>
@@ -30242,7 +30253,7 @@
         <v>0</v>
       </c>
       <c r="AS218" s="55"/>
-      <c r="AT218" s="55"/>
+      <c r="AT218" s="53"/>
       <c r="AU218" s="53">
         <v>265048.72899999999</v>
       </c>
@@ -30356,7 +30367,7 @@
         <v>0</v>
       </c>
       <c r="AS219" s="55"/>
-      <c r="AT219" s="55"/>
+      <c r="AT219" s="53"/>
       <c r="AU219" s="53">
         <v>494018.32400000002</v>
       </c>
@@ -30468,7 +30479,7 @@
         <v>0</v>
       </c>
       <c r="AS220" s="55"/>
-      <c r="AT220" s="55"/>
+      <c r="AT220" s="53"/>
       <c r="AU220" s="53">
         <v>234564.03649999999</v>
       </c>
@@ -30580,7 +30591,7 @@
         <v>0</v>
       </c>
       <c r="AS221" s="55"/>
-      <c r="AT221" s="55"/>
+      <c r="AT221" s="53"/>
       <c r="AU221" s="53">
         <v>236242.68650000001</v>
       </c>
@@ -30690,7 +30701,7 @@
         <v>0</v>
       </c>
       <c r="AS222" s="55"/>
-      <c r="AT222" s="55"/>
+      <c r="AT222" s="53"/>
       <c r="AU222" s="53">
         <v>185875.60550000001</v>
       </c>
@@ -30802,7 +30813,7 @@
         <v>0</v>
       </c>
       <c r="AS223" s="55"/>
-      <c r="AT223" s="55"/>
+      <c r="AT223" s="53"/>
       <c r="AU223" s="53">
         <v>250239.03649999999</v>
       </c>
@@ -30916,7 +30927,7 @@
         <v>0</v>
       </c>
       <c r="AS224" s="55"/>
-      <c r="AT224" s="55"/>
+      <c r="AT224" s="53"/>
       <c r="AU224" s="53">
         <v>244539.03649999999</v>
       </c>
@@ -31030,7 +31041,7 @@
         <v>0</v>
       </c>
       <c r="AS225" s="55"/>
-      <c r="AT225" s="55"/>
+      <c r="AT225" s="53"/>
       <c r="AU225" s="53">
         <v>254989.03649999999</v>
       </c>
@@ -31140,7 +31151,7 @@
         <v>0</v>
       </c>
       <c r="AS226" s="55"/>
-      <c r="AT226" s="55"/>
+      <c r="AT226" s="53"/>
       <c r="AU226" s="53">
         <v>177971.95550000001</v>
       </c>
@@ -31252,7 +31263,7 @@
         <v>23700</v>
       </c>
       <c r="AS227" s="55"/>
-      <c r="AT227" s="55"/>
+      <c r="AT227" s="53"/>
       <c r="AU227" s="53">
         <v>234939.03649999999</v>
       </c>
@@ -31362,7 +31373,7 @@
         <v>0</v>
       </c>
       <c r="AS228" s="55"/>
-      <c r="AT228" s="55"/>
+      <c r="AT228" s="53"/>
       <c r="AU228" s="53">
         <v>236889.03649999999</v>
       </c>
@@ -31474,7 +31485,7 @@
         <v>0</v>
       </c>
       <c r="AS229" s="55"/>
-      <c r="AT229" s="55"/>
+      <c r="AT229" s="53"/>
       <c r="AU229" s="53">
         <v>231664.03649999999</v>
       </c>
@@ -31588,7 +31599,7 @@
         <v>0</v>
       </c>
       <c r="AS230" s="55"/>
-      <c r="AT230" s="55"/>
+      <c r="AT230" s="53"/>
       <c r="AU230" s="53">
         <v>520268.32400000002</v>
       </c>
@@ -31700,7 +31711,7 @@
         <v>0</v>
       </c>
       <c r="AS231" s="55"/>
-      <c r="AT231" s="55"/>
+      <c r="AT231" s="53"/>
       <c r="AU231" s="53">
         <v>525268.32400000002</v>
       </c>
@@ -31812,7 +31823,7 @@
         <v>0</v>
       </c>
       <c r="AS232" s="55"/>
-      <c r="AT232" s="55"/>
+      <c r="AT232" s="53"/>
       <c r="AU232" s="53">
         <v>242892.68650000001</v>
       </c>
@@ -31926,7 +31937,7 @@
         <v>0</v>
       </c>
       <c r="AS233" s="55"/>
-      <c r="AT233" s="55"/>
+      <c r="AT233" s="53"/>
       <c r="AU233" s="53">
         <v>237667.68650000001</v>
       </c>
@@ -32036,7 +32047,7 @@
         <v>0</v>
       </c>
       <c r="AS234" s="55"/>
-      <c r="AT234" s="55"/>
+      <c r="AT234" s="53"/>
       <c r="AU234" s="53">
         <v>189675.60550000001</v>
       </c>
@@ -32148,7 +32159,7 @@
         <v>0</v>
       </c>
       <c r="AS235" s="55"/>
-      <c r="AT235" s="55"/>
+      <c r="AT235" s="53"/>
       <c r="AU235" s="53">
         <v>242417.68650000001</v>
       </c>
@@ -32260,7 +32271,7 @@
         <v>0</v>
       </c>
       <c r="AS236" s="55"/>
-      <c r="AT236" s="55"/>
+      <c r="AT236" s="53"/>
       <c r="AU236" s="53">
         <v>189675.60550000001</v>
       </c>
@@ -32372,7 +32383,7 @@
         <v>0</v>
       </c>
       <c r="AS237" s="55"/>
-      <c r="AT237" s="55"/>
+      <c r="AT237" s="53"/>
       <c r="AU237" s="53">
         <v>242164.03649999999</v>
       </c>
@@ -32484,7 +32495,7 @@
         <v>0</v>
       </c>
       <c r="AS238" s="55"/>
-      <c r="AT238" s="55"/>
+      <c r="AT238" s="53"/>
       <c r="AU238" s="53">
         <v>214596.95550000001</v>
       </c>
@@ -32596,7 +32607,7 @@
         <v>0</v>
       </c>
       <c r="AS239" s="55"/>
-      <c r="AT239" s="55"/>
+      <c r="AT239" s="53"/>
       <c r="AU239" s="53">
         <v>225267.68650000001</v>
       </c>
@@ -32710,7 +32721,7 @@
         <v>0</v>
       </c>
       <c r="AS240" s="55"/>
-      <c r="AT240" s="55"/>
+      <c r="AT240" s="53"/>
       <c r="AU240" s="53">
         <v>239789.03649999999</v>
       </c>
@@ -32822,7 +32833,7 @@
         <v>0</v>
       </c>
       <c r="AS241" s="55"/>
-      <c r="AT241" s="55"/>
+      <c r="AT241" s="53"/>
       <c r="AU241" s="53">
         <v>483768.32400000002</v>
       </c>
@@ -32934,7 +32945,7 @@
         <v>0</v>
       </c>
       <c r="AS242" s="55"/>
-      <c r="AT242" s="55"/>
+      <c r="AT242" s="53"/>
       <c r="AU242" s="53">
         <v>484268.32400000002</v>
       </c>
@@ -33046,7 +33057,7 @@
         <v>0</v>
       </c>
       <c r="AS243" s="55"/>
-      <c r="AT243" s="55"/>
+      <c r="AT243" s="53"/>
       <c r="AU243" s="53">
         <v>256071.92</v>
       </c>
@@ -33156,7 +33167,7 @@
         <v>0</v>
       </c>
       <c r="AS244" s="55"/>
-      <c r="AT244" s="55"/>
+      <c r="AT244" s="53"/>
       <c r="AU244" s="53">
         <v>512268.32400000002</v>
       </c>
@@ -33266,7 +33277,7 @@
         <v>0</v>
       </c>
       <c r="AS245" s="55"/>
-      <c r="AT245" s="55"/>
+      <c r="AT245" s="53"/>
       <c r="AU245" s="53">
         <v>465268.32400000002</v>
       </c>
@@ -33378,7 +33389,7 @@
         <v>7900</v>
       </c>
       <c r="AS246" s="55"/>
-      <c r="AT246" s="55"/>
+      <c r="AT246" s="53"/>
       <c r="AU246" s="53">
         <v>248164.03649999999</v>
       </c>
@@ -33492,7 +33503,7 @@
         <v>0</v>
       </c>
       <c r="AS247" s="55"/>
-      <c r="AT247" s="55"/>
+      <c r="AT247" s="53"/>
       <c r="AU247" s="53">
         <v>237192.68650000001</v>
       </c>
@@ -33604,7 +33615,7 @@
         <v>0</v>
       </c>
       <c r="AS248" s="55"/>
-      <c r="AT248" s="55"/>
+      <c r="AT248" s="53"/>
       <c r="AU248" s="53">
         <v>226071.92</v>
       </c>
@@ -33714,7 +33725,7 @@
         <v>0</v>
       </c>
       <c r="AS249" s="55"/>
-      <c r="AT249" s="55"/>
+      <c r="AT249" s="53"/>
       <c r="AU249" s="53">
         <v>244792.68650000001</v>
       </c>
@@ -33826,7 +33837,7 @@
         <v>0</v>
       </c>
       <c r="AS250" s="55"/>
-      <c r="AT250" s="55"/>
+      <c r="AT250" s="53"/>
       <c r="AU250" s="53">
         <v>217667.68650000001</v>
       </c>
@@ -33940,7 +33951,7 @@
         <v>39500</v>
       </c>
       <c r="AS251" s="55"/>
-      <c r="AT251" s="55"/>
+      <c r="AT251" s="53"/>
       <c r="AU251" s="53">
         <v>265764.03649999999</v>
       </c>
@@ -34052,7 +34063,7 @@
         <v>0</v>
       </c>
       <c r="AS252" s="55"/>
-      <c r="AT252" s="55"/>
+      <c r="AT252" s="53"/>
       <c r="AU252" s="53">
         <v>217192.68650000001</v>
       </c>
@@ -34160,7 +34171,7 @@
         <v>0</v>
       </c>
       <c r="AS253" s="55"/>
-      <c r="AT253" s="55"/>
+      <c r="AT253" s="53"/>
       <c r="AU253" s="53">
         <v>161125.60550000001</v>
       </c>
@@ -34270,7 +34281,7 @@
         <v>15800</v>
       </c>
       <c r="AS254" s="55"/>
-      <c r="AT254" s="55"/>
+      <c r="AT254" s="53"/>
       <c r="AU254" s="53">
         <v>243492.68650000001</v>
       </c>
@@ -34382,7 +34393,7 @@
         <v>0</v>
       </c>
       <c r="AS255" s="55"/>
-      <c r="AT255" s="55"/>
+      <c r="AT255" s="53"/>
       <c r="AU255" s="53">
         <v>226071.92</v>
       </c>
@@ -34494,7 +34505,7 @@
         <v>7900</v>
       </c>
       <c r="AS256" s="55"/>
-      <c r="AT256" s="55"/>
+      <c r="AT256" s="53"/>
       <c r="AU256" s="53">
         <v>429025.60550000001</v>
       </c>
@@ -34604,7 +34615,7 @@
         <v>0</v>
       </c>
       <c r="AS257" s="55"/>
-      <c r="AT257" s="55"/>
+      <c r="AT257" s="53"/>
       <c r="AU257" s="53">
         <v>333412.78146153799</v>
       </c>
@@ -34712,7 +34723,7 @@
         <v>0</v>
       </c>
       <c r="AS258" s="55"/>
-      <c r="AT258" s="55"/>
+      <c r="AT258" s="53"/>
       <c r="AU258" s="53">
         <v>283412.78146153799</v>
       </c>
@@ -34820,7 +34831,7 @@
         <v>0</v>
       </c>
       <c r="AS259" s="55"/>
-      <c r="AT259" s="55"/>
+      <c r="AT259" s="53"/>
       <c r="AU259" s="53">
         <v>177053.94</v>
       </c>
@@ -34924,7 +34935,7 @@
         <v>0</v>
       </c>
       <c r="AS260" s="55"/>
-      <c r="AT260" s="55"/>
+      <c r="AT260" s="53"/>
       <c r="AU260" s="53">
         <v>10000</v>
       </c>
@@ -35028,7 +35039,7 @@
         <v>0</v>
       </c>
       <c r="AS261" s="55"/>
-      <c r="AT261" s="55"/>
+      <c r="AT261" s="53"/>
       <c r="AU261" s="53">
         <v>10000</v>
       </c>
@@ -35134,7 +35145,7 @@
         <v>0</v>
       </c>
       <c r="AS262" s="55"/>
-      <c r="AT262" s="55"/>
+      <c r="AT262" s="53"/>
       <c r="AU262" s="53">
         <v>471268.32400000002</v>
       </c>

</xml_diff>